<commit_message>
Fix answer in Q1. Still need to do the README
</commit_message>
<xml_diff>
--- a/Answers/Gantt.xlsx
+++ b/Answers/Gantt.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Itai\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\מסמכים\לימודים\שנה ב'\סמסטר ב'\67808 - מערכות הפעלה\תרגילים\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -454,8 +454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:P29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -510,37 +510,37 @@
         <v>1</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I10" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J10" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="K10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="L10" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="M10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N10" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>0</v>
       </c>
       <c r="P10" s="6" t="s">
         <v>6</v>
@@ -563,13 +563,13 @@
         <v>8</v>
       </c>
       <c r="F11" s="5">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G11" s="4">
         <v>11</v>
       </c>
       <c r="H11" s="5">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I11" s="5">
         <v>14</v>
@@ -584,7 +584,7 @@
         <v>20</v>
       </c>
       <c r="M11" s="5">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N11" s="5">
         <v>23</v>

</xml_diff>